<commit_message>
Endurance Surface moorings CAL and Ingest
Corrections to Endurance CE07SHSM, CE09OSSM, and CE09OSPM calibration
and ingest csv files.

lat lon format
removed m from depth
added hydrogen sensors to cal sheet
corrected reference designators as necessary
</commit_message>
<xml_diff>
--- a/CE09OSPM/Omaha_Cal_Info_CE09OSPM_00004.xlsx
+++ b/CE09OSPM/Omaha_Cal_Info_CE09OSPM_00004.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\Ingest sheets\ingestion-csvs\CE09OSPM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="12705" yWindow="-15" windowWidth="12510" windowHeight="12405" tabRatio="377" activeTab="1"/>
   </bookViews>
@@ -18,24 +23,24 @@
     <definedName name="_FilterDatabase_0_0_0">Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0_0">Moorings!$A$1:$J$84</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$402</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$401</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$402</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_1">Asset_Cal_Info!$A$1:$F$402</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$401</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_1">Asset_Cal_Info!$A$1:$F$401</definedName>
     <definedName name="_FilterDatabase_0_0_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$F$402</definedName>
+    <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$F$401</definedName>
     <definedName name="_FilterDatabase_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$F$29</definedName>
     <definedName name="_FilterDatabase_1_1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$84</definedName>
-    <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$402</definedName>
+    <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$401</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
   <si>
     <t>Ref Des</t>
   </si>
@@ -161,9 +166,6 @@
   </si>
   <si>
     <t>CC_scattering_angle</t>
-  </si>
-  <si>
-    <t>CE09OSPM-SBS01-00-RTE000000</t>
   </si>
   <si>
     <t>CE09OSPM-WFP01-00-WFPENG000</t>
@@ -217,9 +219,6 @@
   </si>
   <si>
     <t>OSPM-00004-STC</t>
-  </si>
-  <si>
-    <t>OSPM-00004-RTE</t>
   </si>
   <si>
     <t>use adjusted Soc</t>
@@ -606,7 +605,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -641,7 +640,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -853,7 +852,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:M2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -913,7 +912,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="12">
         <v>4</v>
@@ -926,16 +925,16 @@
       </c>
       <c r="F2" s="19"/>
       <c r="G2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="I2" s="5">
         <v>542</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="16">
@@ -963,10 +962,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1017,11 +1016,11 @@
       <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="8" t="s">
-        <v>43</v>
+      <c r="A3" t="s">
+        <v>42</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="9">
         <v>4</v>
@@ -1039,11 +1038,11 @@
       <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="9">
         <v>4</v>
@@ -1059,11 +1058,11 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="9">
         <v>4</v>
@@ -1091,7 +1090,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="9">
         <v>4</v>
@@ -1111,7 +1110,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="9">
         <v>4</v>
@@ -1131,7 +1130,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="9">
         <v>4</v>
@@ -1146,7 +1145,7 @@
         <v>3.2803999999999998E-4</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1154,7 +1153,7 @@
         <v>32</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="9">
         <v>4</v>
@@ -1174,7 +1173,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="9">
         <v>4</v>
@@ -1194,7 +1193,7 @@
         <v>32</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="9">
         <v>4</v>
@@ -1214,7 +1213,7 @@
         <v>32</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="9">
         <v>4</v>
@@ -1234,7 +1233,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="9">
         <v>4</v>
@@ -1262,7 +1261,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="9">
         <v>4</v>
@@ -1277,7 +1276,7 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="G17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1285,7 +1284,7 @@
         <v>34</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="9">
         <v>4</v>
@@ -1305,7 +1304,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="9">
         <v>4</v>
@@ -1325,7 +1324,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="9">
         <v>4</v>
@@ -1345,7 +1344,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="9">
         <v>4</v>
@@ -1365,7 +1364,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="9">
         <v>4</v>
@@ -1385,7 +1384,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="9">
         <v>4</v>
@@ -1405,7 +1404,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="9">
         <v>4</v>
@@ -1425,7 +1424,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="9">
         <v>4</v>
@@ -1445,7 +1444,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="9">
         <v>4</v>
@@ -1473,7 +1472,7 @@
         <v>35</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="9">
         <v>4</v>
@@ -1488,7 +1487,7 @@
         <v>0.9</v>
       </c>
       <c r="G28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1496,7 +1495,7 @@
         <v>35</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="9">
         <v>4</v>
@@ -1511,7 +1510,7 @@
         <v>8.98E-18</v>
       </c>
       <c r="G29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1521,10 +1520,10 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="9">
         <v>4</v>
@@ -1541,10 +1540,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="9">
         <v>4</v>
@@ -1572,33 +1571,16 @@
         <v>36</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="9">
         <v>4</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="9">
-        <v>4</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>